<commit_message>
ignore formula and add DataType::Bool
</commit_message>
<xml_diff>
--- a/tests/issue2.xlsx
+++ b/tests/issue2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,8 +60,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,8 +359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -397,11 +398,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>